<commit_message>
[TID] Add an instruction queue and decouple the fetch unit from the rest of the core
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Instructions</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>InterruptWaits</t>
+  </si>
+  <si>
+    <t>MeanCPI</t>
+  </si>
+  <si>
+    <t>RAM Instructions</t>
+  </si>
+  <si>
+    <t>RAM Instructions Pre HDD</t>
+  </si>
+  <si>
+    <t>Loose Pipeline</t>
+  </si>
+  <si>
+    <t>Loose Pipeline Pre HDD</t>
   </si>
 </sst>
 </file>
@@ -381,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +412,7 @@
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -419,8 +434,11 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -447,19 +465,55 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="e">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="e">
+        <v>2597.1597911227154</v>
+      </c>
+      <c r="C3">
+        <v>4973561</v>
+      </c>
+      <c r="D3">
+        <v>1915</v>
+      </c>
+      <c r="E3">
+        <v>687041</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4278005</v>
+      </c>
+      <c r="H3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2644.2243650047035</v>
+      </c>
+      <c r="C4">
+        <v>5621621</v>
+      </c>
+      <c r="D4">
+        <v>2126</v>
+      </c>
+      <c r="E4">
+        <v>882394</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4729756</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -486,15 +540,255 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="e">
-        <f t="shared" ref="B6:B7" si="1">$C6/$D6</f>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ref="B6:B21" si="1">$C6/$D6</f>
+        <v>2417.877459246768</v>
+      </c>
+      <c r="C6">
+        <v>4301404</v>
+      </c>
+      <c r="D6">
+        <v>1779</v>
+      </c>
+      <c r="E6">
+        <v>482708</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>3811005</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>2488.6767676767677</v>
+      </c>
+      <c r="C7">
+        <v>4927580</v>
+      </c>
+      <c r="D7">
+        <v>1980</v>
+      </c>
+      <c r="E7">
+        <v>677641</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4241346</v>
+      </c>
+      <c r="H7">
+        <v>120</v>
+      </c>
+      <c r="I7">
+        <f>AVERAGE(B2:B7)</f>
+        <v>2562.6001750202036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>374.85396885681735</v>
+      </c>
+      <c r="C9">
+        <v>1973981</v>
+      </c>
+      <c r="D9">
+        <v>5266</v>
+      </c>
+      <c r="E9">
+        <v>612174</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1339927</v>
+      </c>
+      <c r="H9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>266.85506061844433</v>
+      </c>
+      <c r="C10">
+        <v>5876949</v>
+      </c>
+      <c r="D10">
+        <v>22023</v>
+      </c>
+      <c r="E10">
+        <v>811748</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>4976196</v>
+      </c>
+      <c r="H10">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>328.67577155019512</v>
+      </c>
+      <c r="C11">
+        <v>2779611</v>
+      </c>
+      <c r="D11">
+        <v>8457</v>
+      </c>
+      <c r="E11">
+        <v>712522</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2032374</v>
+      </c>
+      <c r="H11">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>301.04762834276789</v>
+      </c>
+      <c r="C12">
+        <v>1542267</v>
+      </c>
+      <c r="D12">
+        <v>5123</v>
+      </c>
+      <c r="E12">
+        <v>409292</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1111908</v>
+      </c>
+      <c r="H12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>248.86225492436361</v>
+      </c>
+      <c r="C13">
+        <v>5445355</v>
+      </c>
+      <c r="D13">
+        <v>21881</v>
+      </c>
+      <c r="E13">
+        <v>608764</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>4748394</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>282.45492889852977</v>
+      </c>
+      <c r="C14">
+        <v>2343811</v>
+      </c>
+      <c r="D14">
+        <v>8298</v>
+      </c>
+      <c r="E14">
+        <v>509112</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1800883</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <f>AVERAGE(B9:B14)</f>
+        <v>300.45826886518637</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="e">
-        <f t="shared" si="1"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f>AVERAGE(B16:B21)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[TID] Add a NOp to remove the single instruction loop, fix counters, empty queue even when waiting for memory
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Instructions</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Loose Pipeline Pre HDD</t>
+  </si>
+  <si>
+    <t>Rogue Instruction Removed</t>
+  </si>
+  <si>
+    <t>Rogue Instruction Removed HDD</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +548,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
-        <f t="shared" ref="B6:B21" si="1">$C6/$D6</f>
+        <f t="shared" ref="B6:B28" si="1">$C6/$D6</f>
         <v>2417.877459246768</v>
       </c>
       <c r="C6">
@@ -750,46 +756,308 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>2.987876158063294</v>
+      </c>
+      <c r="C16">
+        <v>2768085</v>
+      </c>
+      <c r="D16">
+        <v>926439</v>
+      </c>
+      <c r="E16">
+        <v>622526</v>
+      </c>
+      <c r="F16">
+        <v>164</v>
+      </c>
+      <c r="G16">
+        <v>291748</v>
+      </c>
+      <c r="H16">
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>3.4070877131044224</v>
+      </c>
+      <c r="C17">
+        <v>2470527</v>
+      </c>
+      <c r="D17">
+        <v>725114</v>
+      </c>
+      <c r="E17">
+        <v>722729</v>
+      </c>
+      <c r="F17">
+        <v>188</v>
+      </c>
+      <c r="G17">
+        <v>296580</v>
+      </c>
+      <c r="H17">
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>3.0502989383497856</v>
+      </c>
+      <c r="C18">
+        <v>3275411</v>
+      </c>
+      <c r="D18">
+        <v>1073800</v>
+      </c>
+      <c r="E18">
+        <v>823286</v>
+      </c>
+      <c r="F18">
+        <v>220</v>
+      </c>
+      <c r="G18">
+        <v>303451</v>
+      </c>
+      <c r="H18">
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>2.5269203406645961</v>
+      </c>
+      <c r="C19">
+        <v>2340704</v>
+      </c>
+      <c r="D19">
+        <v>926307</v>
+      </c>
+      <c r="E19">
+        <v>418593</v>
+      </c>
+      <c r="F19">
+        <v>80</v>
+      </c>
+      <c r="G19">
+        <v>68854</v>
+      </c>
+      <c r="H19">
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>2.8166907363957754</v>
+      </c>
+      <c r="C20">
+        <v>2042036</v>
+      </c>
+      <c r="D20">
+        <v>724977</v>
+      </c>
+      <c r="E20">
+        <v>518584</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+      <c r="G20">
+        <v>72811</v>
+      </c>
+      <c r="H20">
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>2.6483266846551987</v>
+      </c>
+      <c r="C21">
+        <v>2843368</v>
+      </c>
+      <c r="D21">
+        <v>1073647</v>
+      </c>
+      <c r="E21">
+        <v>618575</v>
+      </c>
+      <c r="F21">
+        <v>120</v>
+      </c>
+      <c r="G21">
+        <v>76768</v>
+      </c>
+      <c r="H21">
+        <v>132</v>
+      </c>
+      <c r="I21">
         <f>AVERAGE(B16:B21)</f>
-        <v>#DIV/0!</v>
+        <v>2.9062000952055116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>317.806378674283</v>
+      </c>
+      <c r="C23">
+        <v>2670527</v>
+      </c>
+      <c r="D23">
+        <v>8403</v>
+      </c>
+      <c r="E23">
+        <v>621514</v>
+      </c>
+      <c r="F23">
+        <v>172</v>
+      </c>
+      <c r="G23">
+        <v>2027926</v>
+      </c>
+      <c r="H23">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>287.52708182476465</v>
+      </c>
+      <c r="C24">
+        <v>3970749</v>
+      </c>
+      <c r="D24">
+        <v>13810</v>
+      </c>
+      <c r="E24">
+        <v>721224</v>
+      </c>
+      <c r="F24">
+        <v>188</v>
+      </c>
+      <c r="G24">
+        <v>3214266</v>
+      </c>
+      <c r="H24">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>299.67006881620659</v>
+      </c>
+      <c r="C25">
+        <v>3875633</v>
+      </c>
+      <c r="D25">
+        <v>12933</v>
+      </c>
+      <c r="E25">
+        <v>821352</v>
+      </c>
+      <c r="F25">
+        <v>220</v>
+      </c>
+      <c r="G25">
+        <v>3021147</v>
+      </c>
+      <c r="H25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>271.27167070217916</v>
+      </c>
+      <c r="C26">
+        <v>2240704</v>
+      </c>
+      <c r="D26">
+        <v>8260</v>
+      </c>
+      <c r="E26">
+        <v>417227</v>
+      </c>
+      <c r="F26">
+        <v>80</v>
+      </c>
+      <c r="G26">
+        <v>1802363</v>
+      </c>
+      <c r="H26">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>259.06955313391353</v>
+      </c>
+      <c r="C27">
+        <v>3542258</v>
+      </c>
+      <c r="D27">
+        <v>13673</v>
+      </c>
+      <c r="E27">
+        <v>517079</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+      <c r="G27">
+        <v>2990497</v>
+      </c>
+      <c r="H27">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>269.45148669796555</v>
+      </c>
+      <c r="C28">
+        <v>3443590</v>
+      </c>
+      <c r="D28">
+        <v>12780</v>
+      </c>
+      <c r="E28">
+        <v>616641</v>
+      </c>
+      <c r="F28">
+        <v>120</v>
+      </c>
+      <c r="G28">
+        <v>2794464</v>
+      </c>
+      <c r="H28">
+        <v>148</v>
+      </c>
+      <c r="I28">
+        <f>AVERAGE(B23:B28)</f>
+        <v>284.13270664155209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[TID] Add loop cache optimisation
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Instructions</t>
   </si>
@@ -63,7 +63,28 @@
     <t>Rogue Instruction Removed</t>
   </si>
   <si>
-    <t>Rogue Instruction Removed HDD</t>
+    <t>Wide Fetch Pre HDD</t>
+  </si>
+  <si>
+    <t>Wide Fetch</t>
+  </si>
+  <si>
+    <t>Rogue Instruction Removed Pre HDD</t>
+  </si>
+  <si>
+    <t>Loop cache</t>
+  </si>
+  <si>
+    <t>Instruction Queue</t>
+  </si>
+  <si>
+    <t>Average Fetch Time</t>
+  </si>
+  <si>
+    <t>Wide Fetch 2</t>
+  </si>
+  <si>
+    <t>Include key loop</t>
   </si>
 </sst>
 </file>
@@ -402,662 +423,1041 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
       <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B4" si="0">$C2/$D2</f>
+        <f t="shared" ref="B2:B7" si="0">$D2/$E2</f>
         <v>2724.789966555184</v>
       </c>
       <c r="C2">
+        <f>$H2/$E2</f>
+        <v>2260.056856187291</v>
+      </c>
+      <c r="D2">
         <v>4073561</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1495</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>687941</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>3378785</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <f t="shared" si="0"/>
         <v>2597.1597911227154</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C39" si="1">$H3/$E3</f>
+        <v>2233.9451697127938</v>
+      </c>
+      <c r="D3">
         <v>4973561</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1915</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>687041</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>4278005</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <f t="shared" si="0"/>
         <v>2644.2243650047035</v>
       </c>
       <c r="C4">
+        <f t="shared" si="1"/>
+        <v>2224.7206020696144</v>
+      </c>
+      <c r="D4">
         <v>5621621</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2126</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>882394</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>4729756</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <f>$C5/$D5</f>
+        <f t="shared" si="0"/>
         <v>2502.8727005150845</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>2142.5938189845474</v>
+      </c>
+      <c r="D5">
         <v>3401404</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1359</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>483608</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>2911785</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
-        <f t="shared" ref="B6:B28" si="1">$C6/$D6</f>
+        <f t="shared" si="0"/>
         <v>2417.877459246768</v>
       </c>
       <c r="C6">
+        <f t="shared" si="1"/>
+        <v>2142.2175379426644</v>
+      </c>
+      <c r="D6">
         <v>4301404</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1779</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>482708</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>3811005</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2488.6767676767677</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2142.0939393939393</v>
+      </c>
+      <c r="D7">
         <v>4927580</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1980</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>677641</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>4241346</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>120</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>AVERAGE(B2:B7)</f>
         <v>2562.6001750202036</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B9:B14" si="2">$D9/$E9</f>
         <v>374.85396885681735</v>
       </c>
       <c r="C9">
+        <f t="shared" si="1"/>
+        <v>254.448727687049</v>
+      </c>
+      <c r="D9">
         <v>1973981</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5266</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>612174</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>1339927</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>266.85506061844433</v>
       </c>
       <c r="C10">
+        <f t="shared" si="1"/>
+        <v>225.95450211142895</v>
+      </c>
+      <c r="D10">
         <v>5876949</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>22023</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>811748</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>4976196</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>328.67577155019512</v>
       </c>
       <c r="C11">
+        <f t="shared" si="1"/>
+        <v>240.31855267825469</v>
+      </c>
+      <c r="D11">
         <v>2779611</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>8457</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>712522</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>2032374</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>301.04762834276789</v>
       </c>
       <c r="C12">
+        <f t="shared" si="1"/>
+        <v>217.04235799336325</v>
+      </c>
+      <c r="D12">
         <v>1542267</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>5123</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>409292</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>1111908</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248.86225492436361</v>
       </c>
       <c r="C13">
+        <f t="shared" si="1"/>
+        <v>217.00991727983182</v>
+      </c>
+      <c r="D13">
         <v>5445355</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>21881</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>608764</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>4748394</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>282.45492889852977</v>
       </c>
       <c r="C14">
+        <f t="shared" si="1"/>
+        <v>217.02615087973007</v>
+      </c>
+      <c r="D14">
         <v>2343811</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>8298</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>509112</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>1800883</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>100</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f>AVERAGE(B9:B14)</f>
         <v>300.45826886518637</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B16:B21" si="3">$D16/$E16</f>
         <v>2.987876158063294</v>
       </c>
       <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.31491334021991735</v>
+      </c>
+      <c r="D16">
         <v>2768085</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>926439</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>622526</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>164</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>291748</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.4070877131044224</v>
       </c>
       <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.40901154852892097</v>
+      </c>
+      <c r="D17">
         <v>2470527</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>725114</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>722729</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>188</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>296580</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.0502989383497856</v>
       </c>
       <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.28259545539206554</v>
+      </c>
+      <c r="D18">
         <v>3275411</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1073800</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>823286</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>220</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>303451</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5269203406645961</v>
       </c>
       <c r="C19">
+        <f t="shared" si="1"/>
+        <v>7.4331728034010322E-2</v>
+      </c>
+      <c r="D19">
         <v>2340704</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>926307</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>418593</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>80</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>68854</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8166907363957754</v>
       </c>
       <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.10043215164067273</v>
+      </c>
+      <c r="D20">
         <v>2042036</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>724977</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>518584</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>100</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>72811</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.6483266846551987</v>
       </c>
       <c r="C21">
+        <f t="shared" si="1"/>
+        <v>7.150208588111362E-2</v>
+      </c>
+      <c r="D21">
         <v>2843368</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>1073647</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>618575</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>120</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>76768</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>132</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f>AVERAGE(B16:B21)</f>
         <v>2.9062000952055116</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B23:B28" si="4">$D23/$E23</f>
         <v>317.806378674283</v>
       </c>
       <c r="C23">
+        <f t="shared" si="1"/>
+        <v>241.33357134356777</v>
+      </c>
+      <c r="D23">
         <v>2670527</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>8403</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>621514</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>172</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>2027926</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>287.52708182476465</v>
       </c>
       <c r="C24">
+        <f t="shared" si="1"/>
+        <v>232.74916727009415</v>
+      </c>
+      <c r="D24">
         <v>3970749</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>13810</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>721224</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>188</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>3214266</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>299.67006881620659</v>
       </c>
       <c r="C25">
+        <f t="shared" si="1"/>
+        <v>233.59986082115518</v>
+      </c>
+      <c r="D25">
         <v>3875633</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>12933</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>821352</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>220</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>3021147</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>271.27167070217916</v>
       </c>
       <c r="C26">
+        <f t="shared" si="1"/>
+        <v>218.20375302663439</v>
+      </c>
+      <c r="D26">
         <v>2240704</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>8260</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>417227</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>80</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>1802363</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>259.06955313391353</v>
       </c>
       <c r="C27">
+        <f t="shared" si="1"/>
+        <v>218.71549769618957</v>
+      </c>
+      <c r="D27">
         <v>3542258</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>13673</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>517079</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>100</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>2990497</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>269.45148669796555</v>
       </c>
       <c r="C28">
+        <f t="shared" si="1"/>
+        <v>218.65915492957745</v>
+      </c>
+      <c r="D28">
         <v>3443590</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>12780</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>616641</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>120</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2794464</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>148</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f>AVERAGE(B23:B28)</f>
         <v>284.13270664155209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <f>$D30/$E30</f>
+        <v>312.13072776280325</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>250.59164420485175</v>
+      </c>
+      <c r="D30">
+        <v>3242414</v>
+      </c>
+      <c r="E30">
+        <v>10388</v>
+      </c>
+      <c r="F30">
+        <v>612902</v>
+      </c>
+      <c r="G30">
+        <v>135</v>
+      </c>
+      <c r="H30">
+        <v>2603146</v>
+      </c>
+      <c r="I30">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <f>$D31/$E31</f>
+        <v>276.04837763878032</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>233.61395621579359</v>
+      </c>
+      <c r="D31">
+        <v>2824527</v>
+      </c>
+      <c r="E31">
+        <v>10232</v>
+      </c>
+      <c r="F31">
+        <v>408330</v>
+      </c>
+      <c r="G31">
+        <v>101</v>
+      </c>
+      <c r="H31">
+        <v>2390338</v>
+      </c>
+      <c r="I31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:B39" si="5">$D33/$E33</f>
+        <v>2457.579250720461</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>2147.242074927954</v>
+      </c>
+      <c r="D33">
+        <v>852780</v>
+      </c>
+      <c r="E33">
+        <v>347</v>
+      </c>
+      <c r="F33">
+        <v>105770</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>745093</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="5"/>
+        <v>254.98847262247838</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>217.62536023054756</v>
+      </c>
+      <c r="D34">
+        <v>88481</v>
+      </c>
+      <c r="E34">
+        <v>347</v>
+      </c>
+      <c r="F34">
+        <v>11120</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>75516</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="5"/>
+        <v>248.57925072046109</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>184.04034582132564</v>
+      </c>
+      <c r="D35">
+        <v>86257</v>
+      </c>
+      <c r="E35">
+        <v>347</v>
+      </c>
+      <c r="F35">
+        <v>21124</v>
+      </c>
+      <c r="G35">
+        <v>28</v>
+      </c>
+      <c r="H35">
+        <v>63862</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="5"/>
+        <v>145.53602305475505</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>108.02593659942363</v>
+      </c>
+      <c r="D36">
+        <v>50501</v>
+      </c>
+      <c r="E36">
+        <v>347</v>
+      </c>
+      <c r="F36">
+        <v>11877</v>
+      </c>
+      <c r="G36">
+        <v>96</v>
+      </c>
+      <c r="H36">
+        <v>37485</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="5"/>
+        <v>141.27953890489914</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>76.858789625360231</v>
+      </c>
+      <c r="D37">
+        <v>49024</v>
+      </c>
+      <c r="E37">
+        <v>347</v>
+      </c>
+      <c r="F37">
+        <v>21136</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <v>26670</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="5"/>
+        <v>43.216138328530256</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>5.3861671469740635</v>
+      </c>
+      <c r="D38">
+        <v>14996</v>
+      </c>
+      <c r="E38">
+        <v>347</v>
+      </c>
+      <c r="F38">
+        <v>12053</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>1869</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="5"/>
+        <v>3.3777788039519834</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>1.3013754699119893E-2</v>
+      </c>
+      <c r="D39">
+        <v>1609238</v>
+      </c>
+      <c r="E39">
+        <v>476419</v>
+      </c>
+      <c r="F39">
+        <v>411728</v>
+      </c>
+      <c r="G39">
+        <v>88</v>
+      </c>
+      <c r="H39">
+        <v>6200</v>
+      </c>
+      <c r="I39">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>